<commit_message>
unlocking locations + failed tool script
</commit_message>
<xml_diff>
--- a/.design/Levels.xlsx
+++ b/.design/Levels.xlsx
@@ -230,61 +230,61 @@
     <t>I like it I think - a decent simple one.</t>
   </si>
   <si>
+    <t>Trickery</t>
+  </si>
+  <si>
+    <t>Also like this one. Plenty of options I think.</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>Maybe. Quite easy I think.</t>
+  </si>
+  <si>
+    <t>Yeah I like this one, just need to rule out alternate paths. Maybe add in some more jumps as red herrings?</t>
+  </si>
+  <si>
+    <t>BadStar</t>
+  </si>
+  <si>
+    <t>Pretty decent easy one.</t>
+  </si>
+  <si>
+    <t>FillipeFilloppe</t>
+  </si>
+  <si>
+    <t>OK I think, will see what the tests show!</t>
+  </si>
+  <si>
+    <t>Twins</t>
+  </si>
+  <si>
+    <t>M/H</t>
+  </si>
+  <si>
+    <t>Decent I think.</t>
+  </si>
+  <si>
+    <t>Mechanisms Included</t>
+  </si>
+  <si>
+    <t>Score, Spring</t>
+  </si>
+  <si>
+    <t>Score, Water</t>
+  </si>
+  <si>
+    <t>Score, Water, Spring</t>
+  </si>
+  <si>
+    <t>Score, Bounce</t>
+  </si>
+  <si>
+    <t>Score, Spring, Water, Bounce</t>
+  </si>
+  <si>
     <t>UpOrDown</t>
-  </si>
-  <si>
-    <t>Trickery</t>
-  </si>
-  <si>
-    <t>Also like this one. Plenty of options I think.</t>
-  </si>
-  <si>
-    <t>EQ</t>
-  </si>
-  <si>
-    <t>Maybe. Quite easy I think.</t>
-  </si>
-  <si>
-    <t>Yeah I like this one, just need to rule out alternate paths. Maybe add in some more jumps as red herrings?</t>
-  </si>
-  <si>
-    <t>BadStar</t>
-  </si>
-  <si>
-    <t>Pretty decent easy one.</t>
-  </si>
-  <si>
-    <t>FillipeFilloppe</t>
-  </si>
-  <si>
-    <t>OK I think, will see what the tests show!</t>
-  </si>
-  <si>
-    <t>Twins</t>
-  </si>
-  <si>
-    <t>M/H</t>
-  </si>
-  <si>
-    <t>Decent I think.</t>
-  </si>
-  <si>
-    <t>Mechanisms Included</t>
-  </si>
-  <si>
-    <t>Score, Spring</t>
-  </si>
-  <si>
-    <t>Score, Water</t>
-  </si>
-  <si>
-    <t>Score, Water, Spring</t>
-  </si>
-  <si>
-    <t>Score, Bounce</t>
-  </si>
-  <si>
-    <t>Score, Spring, Water, Bounce</t>
   </si>
 </sst>
 </file>
@@ -360,9 +360,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -379,6 +376,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2047,15 +2047,15 @@
   <tableColumns count="11">
     <tableColumn id="1" name="Pond" dataDxfId="10"/>
     <tableColumn id="2" name="Stage" dataDxfId="9"/>
-    <tableColumn id="11" name="Mechanisms Included" dataDxfId="0"/>
-    <tableColumn id="3" name="Name" dataDxfId="8"/>
-    <tableColumn id="4" name="Image" dataDxfId="7"/>
-    <tableColumn id="5" name="Score" dataDxfId="6"/>
-    <tableColumn id="6" name="Spring" dataDxfId="5"/>
-    <tableColumn id="7" name="Water" dataDxfId="4"/>
-    <tableColumn id="8" name="Bounce" dataDxfId="3"/>
-    <tableColumn id="9" name="Rating" dataDxfId="2"/>
-    <tableColumn id="10" name="Comments" dataDxfId="1"/>
+    <tableColumn id="11" name="Mechanisms Included" dataDxfId="8"/>
+    <tableColumn id="3" name="Name" dataDxfId="7"/>
+    <tableColumn id="4" name="Image" dataDxfId="6"/>
+    <tableColumn id="5" name="Score" dataDxfId="5"/>
+    <tableColumn id="6" name="Spring" dataDxfId="4"/>
+    <tableColumn id="7" name="Water" dataDxfId="3"/>
+    <tableColumn id="8" name="Bounce" dataDxfId="2"/>
+    <tableColumn id="9" name="Rating" dataDxfId="1"/>
+    <tableColumn id="10" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2327,8 +2327,8 @@
   <dimension ref="B1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2362,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>29</v>
@@ -2477,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
@@ -2641,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
@@ -2768,7 +2768,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>20</v>
@@ -2895,7 +2895,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>26</v>
@@ -2913,7 +2913,7 @@
         <v>43</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2965,10 +2965,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>35</v>
@@ -2980,12 +2980,12 @@
         <v>43</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>35</v>
@@ -2997,7 +2997,7 @@
         <v>42</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
     </row>
     <row r="41" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>35</v>
@@ -3043,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>39</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="44" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>35</v>
@@ -3087,12 +3087,12 @@
         <v>43</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E45" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>35</v>
@@ -3110,27 +3110,27 @@
         <v>43</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K46" s="4" t="s">
+      <c r="L46" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3142,7 @@
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add and editing levels plus fixes
</commit_message>
<xml_diff>
--- a/.design/Levels.xlsx
+++ b/.design/Levels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="93">
   <si>
     <t>Starting Out</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Try and simplify and have no water</t>
   </si>
   <si>
-    <t>Probably not much to do but could do with some final checks</t>
-  </si>
-  <si>
     <t>Quite overwhelming, could probably be omitted for a better design really (or improved)</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Again, limited no. of route options but probably good enough.</t>
   </si>
   <si>
-    <t>Remove the top water tile and this one is good to go.  Probably a good simpler one.</t>
-  </si>
-  <si>
     <t>Good to go.</t>
   </si>
   <si>
@@ -285,6 +279,30 @@
   </si>
   <si>
     <t>UpOrDown</t>
+  </si>
+  <si>
+    <t>SimpleThrough</t>
+  </si>
+  <si>
+    <t>Simplified secondofly</t>
+  </si>
+  <si>
+    <t>Neatened up</t>
+  </si>
+  <si>
+    <t>AFish</t>
+  </si>
+  <si>
+    <t>Wandering</t>
+  </si>
+  <si>
+    <t>Simplified version of Starting out. 20 hop limit so people can just jump around if they want.</t>
+  </si>
+  <si>
+    <t>Allows wandering with 20 hop limit and establishes the fact that you don't always need to get all the scores</t>
+  </si>
+  <si>
+    <t>This one is good to go.  Probably a good simpler one.</t>
   </si>
 </sst>
 </file>
@@ -438,7 +456,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1605791</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1571625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -476,101 +494,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1609385</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="1771650"/>
-          <a:ext cx="1609385" cy="1581150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1606242</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1571625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="3352800"/>
-          <a:ext cx="1606242" cy="1571625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
       <xdr:colOff>1625711</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -587,7 +517,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -608,13 +538,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2131</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -631,7 +561,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -652,13 +582,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1626024</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -675,7 +605,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -696,13 +626,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -719,7 +649,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -740,13 +670,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>64367</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -763,7 +693,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -784,13 +714,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -807,7 +737,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -828,13 +758,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>33083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -851,7 +781,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -872,13 +802,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1581150</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -895,7 +825,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -916,13 +846,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>7486</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -939,7 +869,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -960,13 +890,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1615977</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -983,7 +913,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1004,13 +934,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1599565</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1571625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1027,7 +957,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1048,13 +978,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>23920</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1071,7 +1001,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1092,13 +1022,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1583573</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1115,7 +1045,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1136,13 +1066,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1590675</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>1542473</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1159,7 +1089,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1180,13 +1110,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>5135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1203,7 +1133,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1224,13 +1154,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1588544</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1247,7 +1177,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1268,13 +1198,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1597125</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1562101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1291,7 +1221,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1312,13 +1242,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1579052</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1335,7 +1265,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1356,57 +1286,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1604877</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="46043850"/>
-          <a:ext cx="1604877" cy="1590675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
       <xdr:colOff>1611979</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1423,7 +1309,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1444,13 +1330,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1607344</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1467,7 +1353,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1488,13 +1374,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>7394</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1511,7 +1397,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1532,13 +1418,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1616817</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1555,7 +1441,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1576,13 +1462,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609259</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1599,7 +1485,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1620,13 +1506,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>21453</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1643,7 +1529,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1664,13 +1550,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1687,7 +1573,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1708,13 +1594,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1579145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1731,7 +1617,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1752,13 +1638,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1602517</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1775,7 +1661,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1796,13 +1682,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1595143</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1819,7 +1705,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1840,13 +1726,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1578959</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1863,7 +1749,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1884,13 +1770,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1597125</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>1562101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1907,7 +1793,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1928,13 +1814,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1604877</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1945,7 +1831,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1966,13 +1852,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1602421</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1983,7 +1869,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2004,13 +1890,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2021,7 +1907,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2030,6 +1916,234 @@
         <a:xfrm>
           <a:off x="4667251" y="68370451"/>
           <a:ext cx="1600200" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1614425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372226" y="1962150"/>
+          <a:ext cx="1614424" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1578769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="1962150"/>
+          <a:ext cx="1628775" cy="1578769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619251</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>16887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372226" y="5124450"/>
+          <a:ext cx="1619250" cy="1598037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>26005</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="1962151"/>
+          <a:ext cx="1628775" cy="1607154"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2509</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="5124450"/>
+          <a:ext cx="1631284" cy="1609725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>23643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="41490901"/>
+          <a:ext cx="1619250" cy="1604792"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2042,8 +2156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L46" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B2:L46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L49" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B2:L49"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Pond" dataDxfId="10"/>
     <tableColumn id="2" name="Stage" dataDxfId="9"/>
@@ -2324,11 +2438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L58"/>
+  <dimension ref="B1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2476,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>29</v>
@@ -2389,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="125.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2413,50 +2527,53 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>35</v>
@@ -2464,74 +2581,62 @@
       <c r="K7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
+    </row>
+    <row r="8" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="G8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="125.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>35</v>
@@ -2540,15 +2645,18 @@
         <v>35</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>35</v>
@@ -2557,70 +2665,70 @@
         <v>42</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="15" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>35</v>
@@ -2629,42 +2737,43 @@
         <v>43</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="20" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="I20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>35</v>
@@ -2673,35 +2782,25 @@
         <v>35</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>35</v>
@@ -2716,17 +2815,14 @@
         <v>42</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I24" s="4" t="s">
@@ -2736,12 +2832,12 @@
         <v>42</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>35</v>
@@ -2756,22 +2852,35 @@
         <v>42</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="27" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>35</v>
@@ -2783,12 +2892,12 @@
         <v>42</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>35</v>
@@ -2800,38 +2909,25 @@
         <v>35</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>35</v>
@@ -2840,15 +2936,15 @@
         <v>35</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>35</v>
@@ -2860,15 +2956,15 @@
         <v>35</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>35</v>
@@ -2883,22 +2979,32 @@
         <v>43</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="34" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
-        <v>2</v>
-      </c>
-      <c r="C34" s="1">
-        <v>4</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>35</v>
@@ -2910,15 +3016,15 @@
         <v>35</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>35</v>
@@ -2933,93 +3039,92 @@
         <v>43</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K36" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L36" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L37" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="38" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="1">
-        <v>3</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="H38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="H39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L39" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>35</v>
@@ -3031,37 +3136,38 @@
         <v>43</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="43" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1">
-        <v>3</v>
-      </c>
-      <c r="C43" s="1">
-        <v>2</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>39</v>
+      <c r="E43" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="J43" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>64</v>
@@ -3069,15 +3175,9 @@
     </row>
     <row r="44" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I44" s="4" t="s">
         <v>35</v>
       </c>
       <c r="J44" s="4" t="s">
@@ -3087,74 +3187,130 @@
         <v>43</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L48" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L45" s="8" t="s">
+      <c r="G49" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="1" t="s">
+      <c r="L49" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="1">
+    </row>
+    <row r="50" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
         <v>3</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C51" s="1">
         <v>3</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D51" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
levels + newly activated animation
</commit_message>
<xml_diff>
--- a/.design/Levels.xlsx
+++ b/.design/Levels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
   <si>
     <t>Starting Out</t>
   </si>
@@ -50,9 +50,6 @@
     <t>DoubleJump</t>
   </si>
   <si>
-    <t>WeirdMirror</t>
-  </si>
-  <si>
     <t>Jumpington</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Could do with avoiding the infinite loop black hole.  Might be minor improvements possible.</t>
-  </si>
-  <si>
     <t>Try and simplify and have no water</t>
   </si>
   <si>
@@ -173,12 +167,6 @@
     <t>Probably fine but could do something nice here potentially.</t>
   </si>
   <si>
-    <t>Need to remove the water here</t>
-  </si>
-  <si>
-    <t>Remove the water but otherwise a good one.</t>
-  </si>
-  <si>
     <t>Probably good to go.</t>
   </si>
   <si>
@@ -303,6 +291,21 @@
   </si>
   <si>
     <t>This one is good to go.  Probably a good simpler one.</t>
+  </si>
+  <si>
+    <t>Edgy</t>
+  </si>
+  <si>
+    <t>Worthwhile I think, as need a nicer intro to water</t>
+  </si>
+  <si>
+    <t>Good enough I think</t>
+  </si>
+  <si>
+    <t>WeirdMirror1</t>
+  </si>
+  <si>
+    <t>Might be minor improvements possible.</t>
   </si>
 </sst>
 </file>
@@ -582,234 +585,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1626024</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="11258550"/>
-          <a:ext cx="1626024" cy="1590675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314701" y="12839701"/>
-          <a:ext cx="1638300" cy="1638300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>64367</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314701" y="14420850"/>
-          <a:ext cx="1638300" cy="1645517"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="16002000"/>
-          <a:ext cx="1628775" cy="1628775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>33083</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="17583151"/>
-          <a:ext cx="1628775" cy="1614232"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1581150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1571625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1609726</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -825,15 +608,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="22326600"/>
-          <a:ext cx="1581150" cy="1581150"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="22507575"/>
+          <a:ext cx="1609726" cy="1609726"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -846,13 +629,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>7486</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -869,7 +652,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -890,13 +673,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1615977</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -913,7 +696,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -934,13 +717,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1599565</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1571625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -957,7 +740,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -977,15 +760,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>23920</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>13964</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1571625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1001,35 +784,35 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="31813501"/>
-          <a:ext cx="1652695" cy="1581150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372226" y="30422851"/>
+          <a:ext cx="1642738" cy="1571624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1583573</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>1571625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1621545</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1045,15 +828,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="33394650"/>
-          <a:ext cx="1583573" cy="1590675"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6381750" y="31994475"/>
+          <a:ext cx="1612020" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1066,14 +849,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1590675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1542473</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1786</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1089,15 +872,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="34975800"/>
-          <a:ext cx="1590675" cy="1542473"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="33585150"/>
+          <a:ext cx="1630561" cy="1581150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1111,13 +894,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>5135</xdr:rowOff>
+      <xdr:rowOff>1562100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4679</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1133,15 +916,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="36556950"/>
-          <a:ext cx="1600200" cy="1586285"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="35147250"/>
+          <a:ext cx="1633454" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1155,13 +938,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1588544</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>1552575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1177,15 +960,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="38138100"/>
-          <a:ext cx="1588544" cy="1609725"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="36718875"/>
+          <a:ext cx="1638300" cy="1660144"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1198,14 +981,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1597125</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>1562101</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>21223</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1221,15 +1004,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="39719251"/>
-          <a:ext cx="1597125" cy="1562100"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="38328601"/>
+          <a:ext cx="1638300" cy="1602372"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1242,13 +1025,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1579052</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1265,7 +1048,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1286,13 +1069,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1611979</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1309,7 +1092,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1330,13 +1113,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1607344</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1353,7 +1136,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1374,13 +1157,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>7394</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1397,7 +1180,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1418,13 +1201,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1616817</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1441,7 +1224,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1462,13 +1245,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609259</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1485,7 +1268,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1506,13 +1289,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>21453</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1529,7 +1312,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1550,13 +1333,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1573,7 +1356,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1594,13 +1377,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1579145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1617,7 +1400,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1638,13 +1421,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1602517</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1661,7 +1444,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1682,13 +1465,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1595143</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1705,7 +1488,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1726,13 +1509,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1578959</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1749,7 +1532,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1770,13 +1553,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1597125</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1562101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1793,7 +1576,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1814,13 +1597,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1604877</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1831,7 +1614,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1852,14 +1635,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1602421</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1602421</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1869,7 +1652,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1890,13 +1673,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1600201</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1907,7 +1690,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1945,7 +1728,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1983,7 +1766,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2021,7 +1804,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2059,7 +1842,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2097,7 +1880,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2118,13 +1901,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1619250</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>23643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2135,7 +1918,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2144,6 +1927,234 @@
         <a:xfrm>
           <a:off x="6372225" y="41490901"/>
           <a:ext cx="1619250" cy="1604792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="19354801"/>
+          <a:ext cx="1619250" cy="1597564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1618953</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="11449050"/>
+          <a:ext cx="1618953" cy="1590675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>30935</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="13030200"/>
+          <a:ext cx="1619250" cy="1612085"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>33212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="14611350"/>
+          <a:ext cx="1628775" cy="1614362"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1616849</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372226" y="17773650"/>
+          <a:ext cx="1616848" cy="1609725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1571625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>21379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="16182975"/>
+          <a:ext cx="1619250" cy="1612054"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2156,8 +2167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L49" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B2:L49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B2:L50"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Pond" dataDxfId="10"/>
     <tableColumn id="2" name="Stage" dataDxfId="9"/>
@@ -2438,11 +2449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L61"/>
+  <dimension ref="B1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,42 +2476,42 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="125.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,19 +2522,19 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2534,27 +2545,27 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,24 +2573,24 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,13 +2598,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="125.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2601,13 +2612,13 @@
         <v>3</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2615,13 +2626,13 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2633,22 +2644,22 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2656,16 +2667,16 @@
         <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2673,47 +2684,41 @@
         <v>7</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2725,583 +2730,596 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
-        <v>2</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="H31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="1">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1">
-        <v>4</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E38" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G38" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
         <v>3</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C42" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>42</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>3</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C47" s="1">
         <v>2</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E47" s="1" t="s">
-        <v>66</v>
+      <c r="D47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E48" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E49" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
         <v>3</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C52" s="1">
         <v>3</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D52" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="53" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3311,6 +3329,7 @@
     <row r="59" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:12" ht="125.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>